<commit_message>
Added more tests to excel file
</commit_message>
<xml_diff>
--- a/assign1/ExperimentationResults.xlsx
+++ b/assign1/ExperimentationResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Dropbox\computer\College\Junior\CS492\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Operating-Systems\assign1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9003BDE-526B-4A5E-B09D-A0E17A00C2C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559B4DC7-F912-4B46-88E3-7D77250C08D7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{C05336AD-6F25-424D-B223-C28F3C92E6AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>Test Case</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Seed</t>
   </si>
   <si>
-    <t>FIFO</t>
-  </si>
-  <si>
     <t>RR</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>I pledge my honor that I have abided by the Stevens Honor System.</t>
+  </si>
+  <si>
+    <t>FCFS</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -168,18 +168,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -495,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04933F02-6A3B-4461-B8BD-BF540332EBEB}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +518,7 @@
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,11 +552,38 @@
       <c r="K1" s="1">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="4">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -578,11 +617,38 @@
       <c r="K2">
         <v>5</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>2000</v>
+      </c>
+      <c r="O2">
+        <v>2000</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="T2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -616,8 +682,38 @@
       <c r="K3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>2000</v>
+      </c>
+      <c r="Q3">
+        <v>2000</v>
+      </c>
+      <c r="R3">
+        <v>4</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -651,8 +747,38 @@
       <c r="K4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>100</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4">
+        <v>1000</v>
+      </c>
+      <c r="S4">
+        <v>1000</v>
+      </c>
+      <c r="T4">
+        <v>50</v>
+      </c>
+      <c r="U4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -686,8 +812,38 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -721,8 +877,38 @@
       <c r="K6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>1024</v>
+      </c>
+      <c r="M6">
+        <v>1024</v>
+      </c>
+      <c r="N6">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>1024</v>
+      </c>
+      <c r="Q6">
+        <v>1024</v>
+      </c>
+      <c r="R6">
+        <v>1024</v>
+      </c>
+      <c r="S6">
+        <v>1024</v>
+      </c>
+      <c r="T6">
+        <v>1024</v>
+      </c>
+      <c r="U6">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -756,53 +942,113 @@
       <c r="K7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>123</v>
+      </c>
+      <c r="M7">
+        <v>123</v>
+      </c>
+      <c r="N7">
+        <v>123</v>
+      </c>
+      <c r="O7">
+        <v>123</v>
+      </c>
+      <c r="P7">
+        <v>123</v>
+      </c>
+      <c r="Q7">
+        <v>123</v>
+      </c>
+      <c r="R7">
+        <v>123</v>
+      </c>
+      <c r="S7">
+        <v>123</v>
+      </c>
+      <c r="T7">
+        <v>123</v>
+      </c>
+      <c r="U7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
       <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
       <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
         <v>20</v>
       </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>2187</v>
@@ -834,8 +1080,38 @@
       <c r="K11">
         <v>10829</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>2601</v>
+      </c>
+      <c r="M11">
+        <v>2618</v>
+      </c>
+      <c r="N11">
+        <v>5421</v>
+      </c>
+      <c r="O11">
+        <v>178669</v>
+      </c>
+      <c r="P11">
+        <v>3409</v>
+      </c>
+      <c r="Q11">
+        <v>3404</v>
+      </c>
+      <c r="R11">
+        <v>25805</v>
+      </c>
+      <c r="S11">
+        <v>25485</v>
+      </c>
+      <c r="T11">
+        <v>1361</v>
+      </c>
+      <c r="U11">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -869,8 +1145,38 @@
       <c r="K12">
         <v>8526</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>301</v>
+      </c>
+      <c r="O12">
+        <v>31354</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>3</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -904,8 +1210,38 @@
       <c r="K13">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>53</v>
+      </c>
+      <c r="O13">
+        <v>3571</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -939,8 +1275,38 @@
       <c r="K14">
         <v>3711</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>210</v>
+      </c>
+      <c r="O14">
+        <v>21748</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -974,8 +1340,38 @@
       <c r="K15">
         <v>8524</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>300</v>
+      </c>
+      <c r="O15">
+        <v>31353</v>
+      </c>
+      <c r="P15">
+        <v>9</v>
+      </c>
+      <c r="Q15">
+        <v>11</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1009,8 +1405,38 @@
       <c r="K16">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>52</v>
+      </c>
+      <c r="O16">
+        <v>3571</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1044,8 +1470,38 @@
       <c r="K17">
         <v>3710</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>209</v>
+      </c>
+      <c r="O17">
+        <v>21747</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1079,8 +1535,38 @@
       <c r="K18">
         <v>2989</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>2306</v>
+      </c>
+      <c r="M18">
+        <v>2291</v>
+      </c>
+      <c r="N18">
+        <v>1147</v>
+      </c>
+      <c r="O18">
+        <v>35</v>
+      </c>
+      <c r="P18">
+        <v>1767</v>
+      </c>
+      <c r="Q18">
+        <v>1777</v>
+      </c>
+      <c r="R18">
+        <v>2325</v>
+      </c>
+      <c r="S18">
+        <v>2356</v>
+      </c>
+      <c r="T18">
+        <v>2255</v>
+      </c>
+      <c r="U18">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1114,16 +1600,46 @@
       <c r="K19">
         <v>554</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>2306</v>
+      </c>
+      <c r="M19">
+        <v>2291</v>
+      </c>
+      <c r="N19">
+        <v>1117</v>
+      </c>
+      <c r="O19">
+        <v>35</v>
+      </c>
+      <c r="P19">
+        <v>1760</v>
+      </c>
+      <c r="Q19">
+        <v>1762</v>
+      </c>
+      <c r="R19">
+        <v>2325</v>
+      </c>
+      <c r="S19">
+        <v>2354</v>
+      </c>
+      <c r="T19">
+        <v>2204</v>
+      </c>
+      <c r="U19">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1157,8 +1673,38 @@
       <c r="K22">
         <v>10831</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>2591</v>
+      </c>
+      <c r="M22">
+        <v>2603</v>
+      </c>
+      <c r="N22">
+        <v>5439</v>
+      </c>
+      <c r="O22">
+        <v>178686</v>
+      </c>
+      <c r="P22">
+        <v>3552</v>
+      </c>
+      <c r="Q22">
+        <v>3497</v>
+      </c>
+      <c r="R22">
+        <v>25789</v>
+      </c>
+      <c r="S22">
+        <v>25567</v>
+      </c>
+      <c r="T22">
+        <v>1333</v>
+      </c>
+      <c r="U22">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1192,8 +1738,38 @@
       <c r="K23">
         <v>8724</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>433</v>
+      </c>
+      <c r="O23">
+        <v>31734</v>
+      </c>
+      <c r="P23">
+        <v>11</v>
+      </c>
+      <c r="Q23">
+        <v>11</v>
+      </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
+      <c r="S23">
+        <v>5</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1227,8 +1803,38 @@
       <c r="K24">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>51</v>
+      </c>
+      <c r="O24">
+        <v>3609</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1262,8 +1868,38 @@
       <c r="K25">
         <v>3898</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>247</v>
+      </c>
+      <c r="O25">
+        <v>21931</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>2</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1297,8 +1933,38 @@
       <c r="K26">
         <v>8722</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>433</v>
+      </c>
+      <c r="O26">
+        <v>31731</v>
+      </c>
+      <c r="P26">
+        <v>10</v>
+      </c>
+      <c r="Q26">
+        <v>11</v>
+      </c>
+      <c r="R26">
+        <v>2</v>
+      </c>
+      <c r="S26">
+        <v>5</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1332,8 +1998,38 @@
       <c r="K27">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>50</v>
+      </c>
+      <c r="O27">
+        <v>3609</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1367,8 +2063,38 @@
       <c r="K28">
         <v>3898</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>247</v>
+      </c>
+      <c r="O28">
+        <v>21930</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+      <c r="Q28">
+        <v>2</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>2</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1402,8 +2128,38 @@
       <c r="K29">
         <v>2989</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>2346</v>
+      </c>
+      <c r="M29">
+        <v>2305</v>
+      </c>
+      <c r="N29">
+        <v>1145</v>
+      </c>
+      <c r="O29">
+        <v>35</v>
+      </c>
+      <c r="P29">
+        <v>1696</v>
+      </c>
+      <c r="Q29">
+        <v>1727</v>
+      </c>
+      <c r="R29">
+        <v>2336</v>
+      </c>
+      <c r="S29">
+        <v>2347</v>
+      </c>
+      <c r="T29">
+        <v>2250</v>
+      </c>
+      <c r="U29">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1437,16 +2193,46 @@
       <c r="K30">
         <v>554</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>2315</v>
+      </c>
+      <c r="M30">
+        <v>2305</v>
+      </c>
+      <c r="N30">
+        <v>1111</v>
+      </c>
+      <c r="O30">
+        <v>33</v>
+      </c>
+      <c r="P30">
+        <v>1689</v>
+      </c>
+      <c r="Q30">
+        <v>1715</v>
+      </c>
+      <c r="R30">
+        <v>2326</v>
+      </c>
+      <c r="S30">
+        <v>2346</v>
+      </c>
+      <c r="T30">
+        <v>2250</v>
+      </c>
+      <c r="U30">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -1480,8 +2266,38 @@
       <c r="K33">
         <v>10830</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>2584</v>
+      </c>
+      <c r="M33">
+        <v>2587</v>
+      </c>
+      <c r="N33">
+        <v>5474</v>
+      </c>
+      <c r="O33">
+        <v>178438</v>
+      </c>
+      <c r="P33">
+        <v>3521</v>
+      </c>
+      <c r="Q33">
+        <v>3514</v>
+      </c>
+      <c r="R33">
+        <v>25724</v>
+      </c>
+      <c r="S33">
+        <v>25603</v>
+      </c>
+      <c r="T33">
+        <v>1361</v>
+      </c>
+      <c r="U33">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1515,8 +2331,38 @@
       <c r="K34">
         <v>8723</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>359</v>
+      </c>
+      <c r="O34">
+        <v>31393</v>
+      </c>
+      <c r="P34">
+        <v>6</v>
+      </c>
+      <c r="Q34">
+        <v>11</v>
+      </c>
+      <c r="R34">
+        <v>2</v>
+      </c>
+      <c r="S34">
+        <v>2</v>
+      </c>
+      <c r="T34">
+        <v>2</v>
+      </c>
+      <c r="U34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -1550,8 +2396,38 @@
       <c r="K35">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>51</v>
+      </c>
+      <c r="O35">
+        <v>3539</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1585,8 +2461,38 @@
       <c r="K36">
         <v>3798</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>223</v>
+      </c>
+      <c r="O36">
+        <v>21714</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1620,8 +2526,38 @@
       <c r="K37">
         <v>8722</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>358</v>
+      </c>
+      <c r="O37">
+        <v>31393</v>
+      </c>
+      <c r="P37">
+        <v>6</v>
+      </c>
+      <c r="Q37">
+        <v>11</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <v>2</v>
+      </c>
+      <c r="T37">
+        <v>2</v>
+      </c>
+      <c r="U37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
@@ -1655,8 +2591,38 @@
       <c r="K38">
         <v>101</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>50</v>
+      </c>
+      <c r="O38">
+        <v>3539</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -1690,8 +2656,38 @@
       <c r="K39">
         <v>3797</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>223</v>
+      </c>
+      <c r="O39">
+        <v>21713</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>3</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -1725,8 +2721,38 @@
       <c r="K40">
         <v>2989</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>2321</v>
+      </c>
+      <c r="M40">
+        <v>2319</v>
+      </c>
+      <c r="N40">
+        <v>1148</v>
+      </c>
+      <c r="O40">
+        <v>35</v>
+      </c>
+      <c r="P40">
+        <v>1714</v>
+      </c>
+      <c r="Q40">
+        <v>1714</v>
+      </c>
+      <c r="R40">
+        <v>2341</v>
+      </c>
+      <c r="S40">
+        <v>2343</v>
+      </c>
+      <c r="T40">
+        <v>2204</v>
+      </c>
+      <c r="U40">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1760,16 +2786,46 @@
       <c r="K41">
         <v>554</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>2321</v>
+      </c>
+      <c r="M41">
+        <v>2319</v>
+      </c>
+      <c r="N41">
+        <v>1105</v>
+      </c>
+      <c r="O41">
+        <v>33</v>
+      </c>
+      <c r="P41">
+        <v>1704</v>
+      </c>
+      <c r="Q41">
+        <v>1707</v>
+      </c>
+      <c r="R41">
+        <v>2332</v>
+      </c>
+      <c r="S41">
+        <v>2343</v>
+      </c>
+      <c r="T41">
+        <v>2204</v>
+      </c>
+      <c r="U41">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +2858,7 @@
         <v>60295</v>
       </c>
       <c r="I44">
-        <f t="shared" ref="I44:K44" si="1">AVERAGE(I11,I22,I33)</f>
+        <f t="shared" ref="I44:U44" si="1">AVERAGE(I11,I22,I33)</f>
         <v>343022.66666666669</v>
       </c>
       <c r="J44" s="2">
@@ -1813,8 +2869,48 @@
         <f t="shared" si="1"/>
         <v>10830</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>2592</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="1"/>
+        <v>2602.6666666666665</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="1"/>
+        <v>5444.666666666667</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="1"/>
+        <v>178597.66666666666</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="1"/>
+        <v>3494</v>
+      </c>
+      <c r="Q44" s="2">
+        <f t="shared" si="1"/>
+        <v>3471.6666666666665</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="1"/>
+        <v>25772.666666666668</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="1"/>
+        <v>25551.666666666668</v>
+      </c>
+      <c r="T44" s="2">
+        <f t="shared" si="1"/>
+        <v>1351.6666666666667</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="1"/>
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -1851,15 +2947,55 @@
         <v>1740.3333333333333</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" ref="J45:K45" si="4">AVERAGE(J12,J23,J34)</f>
+        <f t="shared" ref="J45:U45" si="4">AVERAGE(J12,J23,J34)</f>
         <v>2.6666666666666665</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="4"/>
         <v>8657.6666666666661</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L45" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="4"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="4"/>
+        <v>364.33333333333331</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="4"/>
+        <v>31493.666666666668</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="R45" s="2">
+        <f t="shared" si="4"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="T45" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="U45" s="2">
+        <f t="shared" si="4"/>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -1896,15 +3032,55 @@
         <v>102.33333333333333</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:K46" si="6">AVERAGE(J13,J24,J35)</f>
+        <f t="shared" ref="J46:U46" si="6">AVERAGE(J13,J24,J35)</f>
         <v>1</v>
       </c>
       <c r="K46" s="2">
         <f t="shared" si="6"/>
         <v>101.33333333333333</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="6"/>
+        <v>51.666666666666664</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="6"/>
+        <v>3573</v>
+      </c>
+      <c r="P46" s="2">
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Q46" s="2">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R46" s="2">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T46" s="2">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U46" s="2">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -1941,15 +3117,55 @@
         <v>985.33333333333337</v>
       </c>
       <c r="J47">
-        <f t="shared" ref="J47:K47" si="8">AVERAGE(J14,J25,J36)</f>
+        <f t="shared" ref="J47:U47" si="8">AVERAGE(J14,J25,J36)</f>
         <v>1</v>
       </c>
       <c r="K47" s="2">
         <f t="shared" si="8"/>
         <v>3802.3333333333335</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L47" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="8"/>
+        <v>226.66666666666666</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="8"/>
+        <v>21797.666666666668</v>
+      </c>
+      <c r="P47" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="Q47" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T47" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="U47" s="2">
+        <f t="shared" si="8"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
@@ -1986,15 +3202,55 @@
         <v>1740</v>
       </c>
       <c r="J48">
-        <f t="shared" ref="J48:K48" si="10">AVERAGE(J15,J26,J37)</f>
+        <f t="shared" ref="J48:U48" si="10">AVERAGE(J15,J26,J37)</f>
         <v>2</v>
       </c>
       <c r="K48">
         <f t="shared" si="10"/>
         <v>8656</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L48" s="2">
+        <f t="shared" si="10"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="10"/>
+        <v>363.66666666666669</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="10"/>
+        <v>31492.333333333332</v>
+      </c>
+      <c r="P48" s="2">
+        <f t="shared" si="10"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="U48" s="2">
+        <f t="shared" si="10"/>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -2031,15 +3287,55 @@
         <v>102</v>
       </c>
       <c r="J49">
-        <f t="shared" ref="J49:K49" si="12">AVERAGE(J16,J27,J38)</f>
+        <f t="shared" ref="J49:U49" si="12">AVERAGE(J16,J27,J38)</f>
         <v>1</v>
       </c>
       <c r="K49">
         <f t="shared" si="12"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="12"/>
+        <v>50.666666666666664</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="12"/>
+        <v>3573</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>12</v>
       </c>
@@ -2076,15 +3372,55 @@
         <v>984.66666666666663</v>
       </c>
       <c r="J50">
-        <f t="shared" ref="J50:K50" si="14">AVERAGE(J17,J28,J39)</f>
+        <f t="shared" ref="J50:U50" si="14">AVERAGE(J17,J28,J39)</f>
         <v>1</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" si="14"/>
         <v>3801.6666666666665</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="14"/>
+        <v>226.33333333333334</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="14"/>
+        <v>21796.666666666668</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="R50" s="2">
+        <f t="shared" si="14"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="14"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="14"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>13</v>
       </c>
@@ -2121,15 +3457,55 @@
         <v>526</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" ref="J51:K51" si="16">AVERAGE(J18,J29,J40)</f>
+        <f t="shared" ref="J51:U51" si="16">AVERAGE(J18,J29,J40)</f>
         <v>2987.6666666666665</v>
       </c>
       <c r="K51">
         <f t="shared" si="16"/>
         <v>2989</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L51" s="2">
+        <f t="shared" si="16"/>
+        <v>2324.3333333333335</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="16"/>
+        <v>2305</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="16"/>
+        <v>1146.6666666666667</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="P51" s="2">
+        <f t="shared" si="16"/>
+        <v>1725.6666666666667</v>
+      </c>
+      <c r="Q51" s="2">
+        <f t="shared" si="16"/>
+        <v>1739.3333333333333</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="16"/>
+        <v>2334</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="16"/>
+        <v>2348.6666666666665</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="16"/>
+        <v>2236.3333333333335</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="16"/>
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
@@ -2166,15 +3542,65 @@
         <v>524</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" ref="J52:K52" si="18">AVERAGE(J19,J30,J41)</f>
+        <f t="shared" ref="J52:U52" si="18">AVERAGE(J19,J30,J41)</f>
         <v>2971.6666666666665</v>
       </c>
       <c r="K52">
         <f t="shared" si="18"/>
         <v>554</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="L52">
+        <f t="shared" si="18"/>
+        <v>2314</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="18"/>
+        <v>2305</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="18"/>
+        <v>1111</v>
+      </c>
+      <c r="O52" s="2">
+        <f t="shared" si="18"/>
+        <v>33.666666666666664</v>
+      </c>
+      <c r="P52" s="2">
+        <f t="shared" si="18"/>
+        <v>1717.6666666666667</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="18"/>
+        <v>1728</v>
+      </c>
+      <c r="R52" s="2">
+        <f t="shared" si="18"/>
+        <v>2327.6666666666665</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="18"/>
+        <v>2347.6666666666665</v>
+      </c>
+      <c r="T52" s="2">
+        <f t="shared" si="18"/>
+        <v>2219.3333333333335</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="18"/>
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>